<commit_message>
Cadastro de entrada de fornecedores
</commit_message>
<xml_diff>
--- a/Entradas.xlsx
+++ b/Entradas.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,24 +449,49 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>Hora Chegada</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Hora Inicial</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Hora final</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Diferença</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>Observações</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Hora Inicial</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Hora final</t>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Peso Inicial</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Tara</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Peso Final</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Silvio Cesar Junior</t>
+          <t>Junior</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -476,12 +501,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ERU-1020</t>
+          <t>teste-1234</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Logística</t>
+          <t>Produção</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -491,18 +516,43 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Salvando o primeiro ficheiro do dia.
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>04:00</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>
 </t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>19:00</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>19:30</t>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -514,12 +564,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Fornecedor 1</t>
+          <t>Fornecedor 4</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ERU-1000</t>
+          <t>teste-1234</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -529,23 +579,728 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>4561</t>
+          <t>1234</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>
 </t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>14:01</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>16:20</t>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>12kg</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Junior</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Fornecedor 4</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>teste-1234</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Produção</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>12kg</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Junior</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Fornecedor 5</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>teste-1234</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Produção</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>12kg</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Junior</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Fornecedor 6</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>teste-1234</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Produção</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>12kg</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Junior</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Fornecedor 1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>teste-1234</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Produção</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>12kg</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Junior</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Fornecedor 8</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>teste-1234</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Produção</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>12kg</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Junior</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Fornecedor 3</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>teste-1234</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Produção</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>12kg</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Junior</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Fornecedor 7</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>teste-1234</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Produção</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>12kg</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Junior</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Fornecedor 9</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>teste-1234</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Produção</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>12kg</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Junior</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Fornecedor 10</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>teste-1234</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Produção</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>12kg</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Junior</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Fornecedor 11</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>teste-1234</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Produção</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>12kg</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>2kg</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>2kg</t>
         </is>
       </c>
     </row>

</xml_diff>